<commit_message>
a1-update 1901040018 - score in marking file match with error incorrect folder structure
</commit_message>
<xml_diff>
--- a/results/a1/marking-files/a1_1901040018.xlsx
+++ b/results/a1/marking-files/a1_1901040018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mpr\mpr-assignment\a1\marking-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mpr\mpr-spring2023\results\a1\marking-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6D1B2C-E7A0-4A05-A529-C1E435EB78AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F45185-BF2C-4B3F-B1DD-3880A1104826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5505" yWindow="2595" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -722,91 +722,91 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1140,7 +1140,7 @@
       <pane xSplit="8" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,10 +1526,10 @@
       <c r="BX3"/>
     </row>
     <row r="4" spans="2:76" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="69"/>
+      <c r="C4" s="86"/>
       <c r="D4" s="6"/>
       <c r="E4" s="5"/>
       <c r="F4" s="8"/>
@@ -1577,11 +1577,11 @@
       <c r="D6" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="88" t="s">
+      <c r="E6" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
       <c r="H6" s="53" t="s">
         <v>13</v>
       </c>
@@ -1600,16 +1600,16 @@
       <c r="D7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="89" t="s">
+      <c r="E7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
       <c r="H7" s="17">
         <v>5</v>
       </c>
       <c r="I7" s="17">
-        <v>-5</v>
+        <v>-100</v>
       </c>
       <c r="J7" t="s">
         <v>59</v>
@@ -1672,14 +1672,14 @@
     </row>
     <row r="10" spans="2:76" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="90"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
       <c r="I10" s="23"/>
       <c r="BM10"/>
       <c r="BN10"/>
@@ -1696,17 +1696,17 @@
     </row>
     <row r="11" spans="2:76" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
-      <c r="C11" s="93" t="s">
+      <c r="C11" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="91" t="s">
+      <c r="D11" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="87" t="s">
+      <c r="E11" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
       <c r="BM11"/>
@@ -1724,13 +1724,13 @@
     </row>
     <row r="12" spans="2:76" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="74" t="s">
+      <c r="C12" s="73"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
       <c r="H12" s="59">
         <v>2</v>
       </c>
@@ -1750,15 +1750,15 @@
     </row>
     <row r="13" spans="2:76" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
-      <c r="C13" s="94"/>
+      <c r="C13" s="73"/>
       <c r="D13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="74" t="s">
+      <c r="E13" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
       <c r="H13" s="59">
         <v>3</v>
       </c>
@@ -1778,15 +1778,15 @@
     </row>
     <row r="14" spans="2:76" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="82" t="s">
+      <c r="C14" s="73"/>
+      <c r="D14" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="89" t="s">
+      <c r="E14" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
       <c r="H14" s="59">
         <v>5</v>
       </c>
@@ -1806,13 +1806,13 @@
     </row>
     <row r="15" spans="2:76" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="89" t="s">
+      <c r="C15" s="73"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
       <c r="H15" s="59">
         <v>3</v>
       </c>
@@ -1832,15 +1832,15 @@
     </row>
     <row r="16" spans="2:76" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="82" t="s">
+      <c r="C16" s="73"/>
+      <c r="D16" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
       <c r="H16" s="59">
         <v>3</v>
       </c>
@@ -1860,13 +1860,13 @@
     </row>
     <row r="17" spans="1:76" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="67" t="s">
+      <c r="C17" s="73"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
       <c r="H17" s="59">
         <v>3</v>
       </c>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="18" spans="1:76" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="94"/>
+      <c r="C18" s="73"/>
       <c r="D18" s="50"/>
       <c r="E18" s="49"/>
       <c r="F18" s="49"/>
@@ -1908,15 +1908,15 @@
     </row>
     <row r="19" spans="1:76" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
-      <c r="C19" s="94"/>
-      <c r="D19" s="91" t="s">
+      <c r="C19" s="73"/>
+      <c r="D19" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="87" t="s">
+      <c r="E19" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
       <c r="H19" s="60"/>
       <c r="I19" s="60"/>
       <c r="BM19"/>
@@ -1934,13 +1934,13 @@
     </row>
     <row r="20" spans="1:76" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
-      <c r="C20" s="94"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="74" t="s">
+      <c r="C20" s="73"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
       <c r="H20" s="59">
         <v>2</v>
       </c>
@@ -1963,15 +1963,15 @@
         <v>6</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="94"/>
+      <c r="C21" s="73"/>
       <c r="D21" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="74" t="s">
+      <c r="E21" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
       <c r="H21" s="59">
         <v>3</v>
       </c>
@@ -1991,15 +1991,15 @@
     </row>
     <row r="22" spans="1:76" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="82" t="s">
+      <c r="C22" s="73"/>
+      <c r="D22" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="89" t="s">
+      <c r="E22" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
       <c r="H22" s="59">
         <v>5</v>
       </c>
@@ -2019,13 +2019,13 @@
     </row>
     <row r="23" spans="1:76" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="89" t="s">
+      <c r="C23" s="73"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
       <c r="H23" s="59">
         <v>3</v>
       </c>
@@ -2045,15 +2045,15 @@
     </row>
     <row r="24" spans="1:76" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="82" t="s">
+      <c r="C24" s="73"/>
+      <c r="D24" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="67" t="s">
+      <c r="E24" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
       <c r="H24" s="59">
         <v>3</v>
       </c>
@@ -2073,13 +2073,13 @@
     </row>
     <row r="25" spans="1:76" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="67" t="s">
+      <c r="C25" s="73"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
       <c r="H25" s="59">
         <v>3</v>
       </c>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="26" spans="1:76" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
-      <c r="C26" s="94"/>
+      <c r="C26" s="73"/>
       <c r="D26" s="51"/>
       <c r="E26" s="49"/>
       <c r="F26" s="49"/>
@@ -2121,15 +2121,15 @@
     </row>
     <row r="27" spans="1:76" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="83" t="s">
+      <c r="C27" s="73"/>
+      <c r="D27" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="67" t="s">
+      <c r="E27" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
       <c r="H27" s="22">
         <v>3</v>
       </c>
@@ -2149,13 +2149,13 @@
     </row>
     <row r="28" spans="1:76" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="71" t="s">
+      <c r="C28" s="73"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="72"/>
-      <c r="G28" s="73"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="69"/>
       <c r="H28" s="22">
         <v>3</v>
       </c>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="29" spans="1:76" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="71" t="s">
+      <c r="C29" s="74"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="72"/>
-      <c r="G29" s="73"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="69"/>
       <c r="H29" s="22">
         <v>5</v>
       </c>
@@ -2205,11 +2205,11 @@
       <c r="D30" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="71" t="s">
+      <c r="E30" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="72"/>
-      <c r="G30" s="73"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="69"/>
       <c r="H30" s="22">
         <v>0</v>
       </c>
@@ -2273,17 +2273,17 @@
     </row>
     <row r="33" spans="2:76" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
-      <c r="C33" s="85" t="s">
+      <c r="C33" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="82" t="s">
+      <c r="D33" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="67" t="s">
+      <c r="E33" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="22">
         <v>3</v>
       </c>
@@ -2304,13 +2304,13 @@
     </row>
     <row r="34" spans="2:76" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="74" t="s">
+      <c r="C34" s="81"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
       <c r="H34" s="22">
         <v>10</v>
       </c>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="35" spans="2:76" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="75" t="s">
+      <c r="C35" s="81"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
       <c r="H35" s="22">
         <v>5</v>
       </c>
@@ -2356,15 +2356,15 @@
     </row>
     <row r="36" spans="2:76" x14ac:dyDescent="0.25">
       <c r="B36" s="14"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="82" t="s">
+      <c r="C36" s="81"/>
+      <c r="D36" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="76" t="s">
+      <c r="E36" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="77"/>
-      <c r="G36" s="78"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="84"/>
       <c r="H36" s="22">
         <v>3</v>
       </c>
@@ -2384,13 +2384,13 @@
     </row>
     <row r="37" spans="2:76" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="76" t="s">
+      <c r="C37" s="81"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="F37" s="77"/>
-      <c r="G37" s="78"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="84"/>
       <c r="H37" s="22">
         <v>10</v>
       </c>
@@ -2410,13 +2410,13 @@
     </row>
     <row r="38" spans="2:76" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="84"/>
-      <c r="E38" s="67" t="s">
+      <c r="C38" s="81"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="79"/>
       <c r="H38" s="22">
         <v>5</v>
       </c>
@@ -2438,9 +2438,9 @@
       <c r="B39" s="14"/>
       <c r="C39" s="24"/>
       <c r="D39" s="16"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="67"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="79"/>
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
       <c r="BM39"/>
@@ -2480,17 +2480,17 @@
     </row>
     <row r="41" spans="2:76" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="14"/>
-      <c r="C41" s="85" t="s">
+      <c r="C41" s="80" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="71" t="s">
+      <c r="E41" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="F41" s="72"/>
-      <c r="G41" s="73"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="69"/>
       <c r="H41" s="22">
         <v>5</v>
       </c>
@@ -2510,15 +2510,15 @@
     </row>
     <row r="42" spans="2:76" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="14"/>
-      <c r="C42" s="86"/>
+      <c r="C42" s="81"/>
       <c r="D42" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="79" t="s">
+      <c r="E42" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="F42" s="80"/>
-      <c r="G42" s="81"/>
+      <c r="F42" s="94"/>
+      <c r="G42" s="95"/>
       <c r="H42" s="22">
         <v>2</v>
       </c>
@@ -2538,8 +2538,8 @@
     </row>
     <row r="43" spans="2:76" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="14"/>
-      <c r="C43" s="86"/>
-      <c r="D43" s="82" t="s">
+      <c r="C43" s="81"/>
+      <c r="D43" s="75" t="s">
         <v>25</v>
       </c>
       <c r="E43" t="s">
@@ -2564,13 +2564,13 @@
     </row>
     <row r="44" spans="2:76" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="14"/>
-      <c r="C44" s="86"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="71" t="s">
+      <c r="C44" s="81"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="F44" s="72"/>
-      <c r="G44" s="73"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="69"/>
       <c r="H44" s="22">
         <v>3</v>
       </c>
@@ -2639,17 +2639,17 @@
       <c r="BX47"/>
     </row>
     <row r="48" spans="2:76" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="68" t="s">
+      <c r="B48" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="68"/>
+      <c r="C48" s="91"/>
       <c r="H48" s="35">
         <f>SUM(H7:H45)</f>
         <v>100</v>
       </c>
       <c r="I48" s="35">
         <f>100+SUM(I7:I44)</f>
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="BM48"/>
       <c r="BN48"/>
@@ -2679,10 +2679,10 @@
       <c r="BX49"/>
     </row>
     <row r="50" spans="2:110" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="69" t="s">
+      <c r="B50" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="69"/>
+      <c r="C50" s="86"/>
       <c r="BM50"/>
       <c r="BN50"/>
       <c r="BO50"/>
@@ -2844,13 +2844,45 @@
     </row>
     <row r="58" spans="2:110" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="2:110" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="70" t="s">
+      <c r="B59" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="70"/>
+      <c r="C59" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E19:G19"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="D27:D29"/>
     <mergeCell ref="C11:C29"/>
@@ -2867,38 +2899,6 @@
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:G28"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E38:G38"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:I44">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">

</xml_diff>